<commit_message>
updates on new setup
</commit_message>
<xml_diff>
--- a/docs/demo/microscope_camera_20X_4X_3_5X_calibration.xlsx
+++ b/docs/demo/microscope_camera_20X_4X_3_5X_calibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utkug\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnmi223\Documents\SLMeasure\docs\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82478445-0726-403F-BC4C-8CC66474AD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D12FBF-40A4-457D-BC69-C1E421DCB465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="3765" windowWidth="20400" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -6087,8 +6087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83697F2B-EC02-4AC4-AFB2-EF9B1654260C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6117,7 +6117,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.28660000000000002</v>
+        <v>0.31950000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6320,7 +6320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -6803,6 +6803,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13231beaf431ebcd1e0feea1ee7400a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c43bb9650fad45b6068276d37b57855" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -7045,16 +7054,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F086F28B-3FFC-4AC1-9335-7C0762A8A930}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09719283-347B-4264-89DE-D5D1CB5B0CE5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7071,12 +7079,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F086F28B-3FFC-4AC1-9335-7C0762A8A930}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>